<commit_message>
Move logIn method back to BaseTest, add priority to login tests
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djoshke\IdeaProjects\qa-itbootcamp-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06926B28-732B-49AC-8C76-D6DD28D7B2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A3E0B-E555-46E6-9958-7EAD84B9F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Valid username</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>/static/media/red-tatt-1200x1500.30dadef4.jpg</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>nonstandard_user6</t>
+  </si>
+  <si>
+    <t>public_sauce6</t>
   </si>
 </sst>
 </file>
@@ -435,10 +444,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -533,6 +542,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -543,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12966EB7-D1AD-48F2-BA9D-4CEFF6017738}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change login case sensitivity tests to match manual test cases text
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djoshke\IdeaProjects\qa-itbootcamp-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A3E0B-E555-46E6-9958-7EAD84B9F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15024856-4A24-4EA6-84E4-C2CDAC0782F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Valid username</t>
   </si>
@@ -148,15 +148,6 @@
   </si>
   <si>
     <t>/static/media/red-tatt-1200x1500.30dadef4.jpg</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>nonstandard_user6</t>
-  </si>
-  <si>
-    <t>public_sauce6</t>
   </si>
 </sst>
 </file>
@@ -444,10 +435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -458,7 +449,7 @@
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -486,7 +477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -500,7 +491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -514,7 +505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -528,7 +519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -540,20 +531,6 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start inventory page tests
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djoshke\IdeaProjects\qa-itbootcamp-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15024856-4A24-4EA6-84E4-C2CDAC0782F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7871C0-DA11-41AF-ADEE-54B87465FC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="3675" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,6 +215,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -437,7 +440,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -543,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12966EB7-D1AD-48F2-BA9D-4CEFF6017738}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -552,7 +555,7 @@
     <col min="1" max="1" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="48.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="49" style="3"/>
   </cols>
@@ -564,7 +567,7 @@
       <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -581,7 +584,7 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>29.99</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -599,7 +602,7 @@
       <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>9.99</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -616,7 +619,7 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>15.99</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -633,7 +636,7 @@
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>49.99</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -650,7 +653,7 @@
       <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>7.99</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -667,7 +670,7 @@
       <c r="C7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="5">
         <v>15.99</v>
       </c>
       <c r="E7" s="4" t="s">

</xml_diff>

<commit_message>
Add function to get data from excel, locator names
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djoshke\IdeaProjects\qa-itbootcamp-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7871C0-DA11-41AF-ADEE-54B87465FC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E17610-C7DD-41EF-9630-9A8A2135CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="3675" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Valid username</t>
   </si>
@@ -148,13 +148,28 @@
   </si>
   <si>
     <t>/static/media/red-tatt-1200x1500.30dadef4.jpg</t>
+  </si>
+  <si>
+    <t>29.99</t>
+  </si>
+  <si>
+    <t>9.99</t>
+  </si>
+  <si>
+    <t>15.99</t>
+  </si>
+  <si>
+    <t>49.99</t>
+  </si>
+  <si>
+    <t>7.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -186,6 +201,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -218,6 +239,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -547,7 +571,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -555,7 +579,7 @@
     <col min="1" max="1" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="48.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="49" style="3"/>
   </cols>
@@ -584,8 +608,8 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5">
-        <v>29.99</v>
+      <c r="D2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>26</v>
@@ -602,11 +626,14 @@
       <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5">
-        <v>9.99</v>
+      <c r="D3" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="F3" s="5">
+        <v>9.99</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -619,11 +646,14 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="5">
-        <v>15.99</v>
+      <c r="D4" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>38</v>
+      </c>
+      <c r="F4" s="5">
+        <v>15.99</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -636,11 +666,14 @@
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="5">
-        <v>49.99</v>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="F5" s="5">
+        <v>49.99</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
@@ -653,11 +686,14 @@
       <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="5">
-        <v>7.99</v>
+      <c r="D6" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="F6" s="5">
+        <v>7.99</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -670,14 +706,18 @@
       <c r="C7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="5">
-        <v>15.99</v>
+      <c r="D7" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="F7" s="5">
+        <v>15.99</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>